<commit_message>
Updated to check SCE expenses
</commit_message>
<xml_diff>
--- a/datafiles/all_td_expense_cols.xlsx
+++ b/datafiles/all_td_expense_cols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rayan/Developer/UtilExpenses/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47E37D30-2A21-7844-BE5C-4511248D3CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AC45B4-796A-AF48-9F0B-DDE50E21BA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="13660" xr2:uid="{C8D8D7EA-67E4-5A4B-BE49-FFB73C837986}"/>
+    <workbookView xWindow="10980" yWindow="1000" windowWidth="14540" windowHeight="13660" xr2:uid="{C8D8D7EA-67E4-5A4B-BE49-FFB73C837986}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -606,8 +606,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -635,8 +643,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -953,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F895E5-39FA-304C-AD53-63188DF3214B}">
   <dimension ref="A1:A188"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="A26" sqref="A21:A26"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1268,17 +1277,17 @@
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1318,7 +1327,7 @@
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1338,7 +1347,7 @@
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1363,7 +1372,7 @@
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1388,7 +1397,7 @@
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1398,7 +1407,7 @@
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1904,5 +1913,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added data request files
</commit_message>
<xml_diff>
--- a/datafiles/all_td_expense_cols.xlsx
+++ b/datafiles/all_td_expense_cols.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rayan/Developer/UtilExpenses/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AC45B4-796A-AF48-9F0B-DDE50E21BA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0770C52-2353-7349-BA12-D548A95DF4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10980" yWindow="1000" windowWidth="14540" windowHeight="13660" xr2:uid="{C8D8D7EA-67E4-5A4B-BE49-FFB73C837986}"/>
+    <workbookView xWindow="0" yWindow="1340" windowWidth="25520" windowHeight="13660" xr2:uid="{C8D8D7EA-67E4-5A4B-BE49-FFB73C837986}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -643,9 +643,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -962,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F895E5-39FA-304C-AD53-63188DF3214B}">
   <dimension ref="A1:A188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="138" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -982,7 +983,7 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -992,7 +993,7 @@
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1077,22 +1078,22 @@
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1172,7 +1173,7 @@
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1352,7 +1353,7 @@
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1392,7 +1393,7 @@
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1402,17 +1403,17 @@
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1532,12 +1533,12 @@
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+      <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+      <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1547,12 +1548,12 @@
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+      <c r="A116" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+      <c r="A117" s="1" t="s">
         <v>116</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated graphs to add SCE distr components, updated data with new pudl.sqlite
</commit_message>
<xml_diff>
--- a/datafiles/all_td_expense_cols.xlsx
+++ b/datafiles/all_td_expense_cols.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rayan/Developer/UtilExpenses/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0770C52-2353-7349-BA12-D548A95DF4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27939B93-D83A-C542-B8D3-EB4A4857BDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1340" windowWidth="25520" windowHeight="13660" xr2:uid="{C8D8D7EA-67E4-5A4B-BE49-FFB73C837986}"/>
+    <workbookView xWindow="0" yWindow="960" windowWidth="10820" windowHeight="13660" xr2:uid="{C8D8D7EA-67E4-5A4B-BE49-FFB73C837986}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -606,7 +606,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -616,6 +616,23 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -643,10 +660,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -963,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F895E5-39FA-304C-AD53-63188DF3214B}">
   <dimension ref="A1:A188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="138" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A69" activeCellId="8" sqref="A51 A53 A48 A85 A89 A71 A73 A87 A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1148,7 +1166,7 @@
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1178,17 +1196,17 @@
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="A44" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1333,7 +1351,7 @@
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="A73" s="3" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1408,7 +1426,7 @@
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
+      <c r="A88" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1503,7 +1521,7 @@
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="A107" s="3" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1553,7 +1571,7 @@
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
+      <c r="A117" s="2" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1628,12 +1646,12 @@
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
+      <c r="A132" s="3" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
+      <c r="A133" s="3" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1708,12 +1726,12 @@
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
+      <c r="A148" s="3" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
+      <c r="A149" s="3" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1753,7 +1771,7 @@
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
+      <c r="A157" s="3" t="s">
         <v>156</v>
       </c>
     </row>
@@ -1768,7 +1786,7 @@
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
+      <c r="A160" s="3" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1778,7 +1796,7 @@
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
+      <c r="A162" s="3" t="s">
         <v>161</v>
       </c>
     </row>
@@ -1868,7 +1886,7 @@
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A180" t="s">
+      <c r="A180" s="3" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1888,7 +1906,7 @@
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
+      <c r="A184" s="3" t="s">
         <v>183</v>
       </c>
     </row>
@@ -1903,7 +1921,7 @@
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A187" t="s">
+      <c r="A187" s="3" t="s">
         <v>186</v>
       </c>
     </row>

</xml_diff>